<commit_message>
updated everything with new infur data
</commit_message>
<xml_diff>
--- a/www/data/BirdlistI.xlsx
+++ b/www/data/BirdlistI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/marcel_klaassen_deakin_edu_au/Documents/Active projects/Em/AIV panzootic/R/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/marcel_klaassen_deakin_edu_au/Documents/Active projects/Influenza/HPAI H5 mapping project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{CBEB85B0-86C8-47FD-A8EB-F2B2EA4AA276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF757E65-DC1E-4E47-9B0F-D89B42988DBF}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="13_ncr:1_{CBEB85B0-86C8-47FD-A8EB-F2B2EA4AA276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01DA5299-E820-4ABD-AB0E-8456C58F52ED}"/>
   <bookViews>
-    <workbookView xWindow="31095" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3510" windowWidth="28800" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BirdlistI" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="752">
   <si>
     <t>Corvus frugilegus</t>
   </si>
@@ -2250,13 +2250,55 @@
   </si>
   <si>
     <t>Picidae</t>
+  </si>
+  <si>
+    <t>Accipiter trinotatus</t>
+  </si>
+  <si>
+    <t>Felis silvestris</t>
+  </si>
+  <si>
+    <t>Sciurus carolinensis</t>
+  </si>
+  <si>
+    <t>Procellariidae (incognita)</t>
+  </si>
+  <si>
+    <t>Aegypius monachus</t>
+  </si>
+  <si>
+    <t>Mustela erminea</t>
+  </si>
+  <si>
+    <t>Leucophaeus scoresbii</t>
+  </si>
+  <si>
+    <t>Anas georgica</t>
+  </si>
+  <si>
+    <t>Theristicus melanopis</t>
+  </si>
+  <si>
+    <t>Pelecanoides garnotii</t>
+  </si>
+  <si>
+    <t>Oceanites oceanicus</t>
+  </si>
+  <si>
+    <t>Bubo magellanicus</t>
+  </si>
+  <si>
+    <t>Procellariidae</t>
+  </si>
+  <si>
+    <t>Oceanitidae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2410,6 +2452,12 @@
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF474747"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2759,7 +2807,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2775,6 +2823,7 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3130,11 +3179,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G599"/>
+  <dimension ref="A1:G611"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I597" sqref="I597"/>
+      <pane ySplit="1" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C584" sqref="C584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15309,6 +15358,270 @@
         <v>0</v>
       </c>
     </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>738</v>
+      </c>
+      <c r="B600" t="s">
+        <v>406</v>
+      </c>
+      <c r="C600" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D600" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="E600" t="s">
+        <v>738</v>
+      </c>
+      <c r="F600">
+        <v>0</v>
+      </c>
+      <c r="G600">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>739</v>
+      </c>
+      <c r="B601" t="s">
+        <v>698</v>
+      </c>
+      <c r="C601" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D601" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="F601">
+        <v>0</v>
+      </c>
+      <c r="G601">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>740</v>
+      </c>
+      <c r="B602" t="s">
+        <v>698</v>
+      </c>
+      <c r="C602" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="D602" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="F602">
+        <v>0</v>
+      </c>
+      <c r="G602">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>741</v>
+      </c>
+      <c r="B603" t="s">
+        <v>406</v>
+      </c>
+      <c r="C603" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D603" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="F603">
+        <v>1</v>
+      </c>
+      <c r="G603">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>742</v>
+      </c>
+      <c r="B604" t="s">
+        <v>406</v>
+      </c>
+      <c r="C604" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D604" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="E604" t="s">
+        <v>742</v>
+      </c>
+      <c r="F604">
+        <v>0</v>
+      </c>
+      <c r="G604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>743</v>
+      </c>
+      <c r="B605" t="s">
+        <v>698</v>
+      </c>
+      <c r="C605" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D605" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="F605">
+        <v>0</v>
+      </c>
+      <c r="G605">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>744</v>
+      </c>
+      <c r="B606" t="s">
+        <v>406</v>
+      </c>
+      <c r="C606" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D606" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="E606" t="s">
+        <v>744</v>
+      </c>
+      <c r="F606">
+        <v>1</v>
+      </c>
+      <c r="G606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>745</v>
+      </c>
+      <c r="B607" t="s">
+        <v>406</v>
+      </c>
+      <c r="C607" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D607" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E607" t="s">
+        <v>745</v>
+      </c>
+      <c r="F607">
+        <v>0</v>
+      </c>
+      <c r="G607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>746</v>
+      </c>
+      <c r="B608" t="s">
+        <v>406</v>
+      </c>
+      <c r="C608" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D608" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="E608" t="s">
+        <v>746</v>
+      </c>
+      <c r="F608">
+        <v>0</v>
+      </c>
+      <c r="G608">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>747</v>
+      </c>
+      <c r="B609" t="s">
+        <v>406</v>
+      </c>
+      <c r="C609" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D609" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="E609" t="s">
+        <v>747</v>
+      </c>
+      <c r="F609">
+        <v>1</v>
+      </c>
+      <c r="G609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>748</v>
+      </c>
+      <c r="B610" t="s">
+        <v>406</v>
+      </c>
+      <c r="C610" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D610" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="E610" t="s">
+        <v>748</v>
+      </c>
+      <c r="F610">
+        <v>1</v>
+      </c>
+      <c r="G610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>749</v>
+      </c>
+      <c r="B611" t="s">
+        <v>406</v>
+      </c>
+      <c r="C611" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D611" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E611" t="s">
+        <v>749</v>
+      </c>
+      <c r="F611">
+        <v>0</v>
+      </c>
+      <c r="G611">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G589">
     <sortCondition descending="1" ref="B2:B589"/>

</xml_diff>

<commit_message>
updated with WOAH 28 April 2025 data
</commit_message>
<xml_diff>
--- a/www/data/BirdlistI.xlsx
+++ b/www/data/BirdlistI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/marcel_klaassen_deakin_edu_au/Documents/Active projects/Influenza/HPAI H5 mapping project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deakin365-my.sharepoint.com/personal/marcel_klaassen_deakin_edu_au/Documents/Active projects/Github/HPAI_RiskMapping_Dashboard/www/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="13_ncr:1_{CBEB85B0-86C8-47FD-A8EB-F2B2EA4AA276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01DA5299-E820-4ABD-AB0E-8456C58F52ED}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{CBEB85B0-86C8-47FD-A8EB-F2B2EA4AA276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86C34F04-99D2-4DCA-B4DC-44643B47538B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3510" windowWidth="28800" windowHeight="11415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22770" yWindow="1545" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BirdlistI" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2457" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2472" uniqueCount="755">
   <si>
     <t>Corvus frugilegus</t>
   </si>
@@ -2292,13 +2292,22 @@
   </si>
   <si>
     <t>Oceanitidae</t>
+  </si>
+  <si>
+    <t>Hieraaetus pennatus</t>
+  </si>
+  <si>
+    <t>Accipiter novaehollandiae</t>
+  </si>
+  <si>
+    <t>Accipiter poliocephalus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2458,6 +2467,13 @@
       <color rgb="FF474747"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2807,7 +2823,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2824,6 +2840,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3179,11 +3198,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G611"/>
+  <dimension ref="A1:G614"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A531" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C584" sqref="C584"/>
+      <pane ySplit="1" topLeftCell="A606" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F615" sqref="F615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15622,6 +15641,75 @@
         <v>0</v>
       </c>
     </row>
+    <row r="612" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A612" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="B612" t="s">
+        <v>406</v>
+      </c>
+      <c r="C612" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D612" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="E612" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="F612">
+        <v>0</v>
+      </c>
+      <c r="G612">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>753</v>
+      </c>
+      <c r="B613" t="s">
+        <v>406</v>
+      </c>
+      <c r="C613" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D613" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="E613" t="s">
+        <v>753</v>
+      </c>
+      <c r="F613">
+        <v>0</v>
+      </c>
+      <c r="G613">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="614" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>754</v>
+      </c>
+      <c r="B614" t="s">
+        <v>406</v>
+      </c>
+      <c r="C614" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D614" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="E614" t="s">
+        <v>754</v>
+      </c>
+      <c r="F614">
+        <v>0</v>
+      </c>
+      <c r="G614">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G589">
     <sortCondition descending="1" ref="B2:B589"/>

</xml_diff>